<commit_message>
Matching category codes under progress
</commit_message>
<xml_diff>
--- a/Data/Product_categories.xlsx
+++ b/Data/Product_categories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/bertiner_ntnu_no/Documents/2_Env_Eng/IOA_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="512" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5783A8D0-6FC0-4EA7-A35F-8EF3819EBE0C}"/>
+  <xr:revisionPtr revIDLastSave="513" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0743F57-FA8F-4F9E-A3B0-60AECAF42C30}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -278,7 +278,7 @@
     <t>Public administration and defense services</t>
   </si>
   <si>
-    <t>Products of vegetable oils and fats</t>
+    <t>Products of Vegetable oils and fats</t>
   </si>
   <si>
     <t>Renting services of machinery and equipment without operator and of personal and household goods</t>
@@ -353,9 +353,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,351 +692,350 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40" style="1" customWidth="1"/>
-    <col min="2" max="2" width="66.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="47.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="60.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="37" style="1" customWidth="1"/>
-    <col min="8" max="8" width="31" style="1" customWidth="1"/>
-    <col min="9" max="9" width="35.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="103.7109375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="2" width="66.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="47.42578125" customWidth="1"/>
+    <col min="5" max="5" width="60.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" customWidth="1"/>
+    <col min="7" max="7" width="37" customWidth="1"/>
+    <col min="8" max="8" width="31" customWidth="1"/>
+    <col min="9" max="9" width="35.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" customWidth="1"/>
+    <col min="12" max="12" width="103.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" t="s">
         <v>42</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" t="s">
         <v>48</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" t="s">
         <v>54</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>59</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" t="s">
         <v>60</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" t="s">
         <v>65</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>69</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" t="s">
         <v>70</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L9" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>73</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L10" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>76</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L11" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>78</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L12" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>80</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="L13" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>82</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="L14" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>84</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="L15" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="L16" s="1" t="s">
+      <c r="L16" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="17" spans="12:12">
-      <c r="L17" s="1" t="s">
+      <c r="L17" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="18" spans="12:12">
-      <c r="L18" s="1" t="s">
+      <c r="L18" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="12:12">
-      <c r="L19" s="1" t="s">
+      <c r="L19" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="20" spans="12:12">
-      <c r="L20" s="1" t="s">
+      <c r="L20" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="21" spans="12:12">
-      <c r="L21" s="1" t="s">
+      <c r="L21" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="22" spans="12:12">
-      <c r="L22" s="1" t="s">
+      <c r="L22" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="23" spans="12:12">
-      <c r="L23" s="1" t="s">
+      <c r="L23" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding expences, doing some testing
</commit_message>
<xml_diff>
--- a/Data/Product_categories.xlsx
+++ b/Data/Product_categories.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27612"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/bertiner_ntnu_no/Documents/2_Env_Eng/IOA_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="513" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0743F57-FA8F-4F9E-A3B0-60AECAF42C30}"/>
+  <xr:revisionPtr revIDLastSave="557" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEC0D3A0-7625-4123-BA59-2724C1C7BAF0}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,42 +36,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
-  <si>
-    <t>[CP01]</t>
-  </si>
-  <si>
-    <t>[CP02]</t>
-  </si>
-  <si>
-    <t>[CP03]</t>
-  </si>
-  <si>
-    <t>[CP04]</t>
-  </si>
-  <si>
-    <t>[CP05]</t>
-  </si>
-  <si>
-    <t>[CP06]</t>
-  </si>
-  <si>
-    <t>[CP07]</t>
-  </si>
-  <si>
-    <t>[CP08]</t>
-  </si>
-  <si>
-    <t>[CP09]</t>
-  </si>
-  <si>
-    <t>[CP10]</t>
-  </si>
-  <si>
-    <t>[CP11]</t>
-  </si>
-  <si>
-    <t>[CP12]</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="114">
+  <si>
+    <t>CP01</t>
+  </si>
+  <si>
+    <t>CP02</t>
+  </si>
+  <si>
+    <t>CP03</t>
+  </si>
+  <si>
+    <t>CP04</t>
+  </si>
+  <si>
+    <t>CP05</t>
+  </si>
+  <si>
+    <t>CP06</t>
+  </si>
+  <si>
+    <t>CP07</t>
+  </si>
+  <si>
+    <t>CP08</t>
+  </si>
+  <si>
+    <t>CP09</t>
+  </si>
+  <si>
+    <t>CP10</t>
+  </si>
+  <si>
+    <t>CP11</t>
+  </si>
+  <si>
+    <t>CP12</t>
   </si>
   <si>
     <t>Food and non-alcoholic beverages</t>
@@ -110,224 +110,333 @@
     <t>Miscellaneous goods and services</t>
   </si>
   <si>
-    <t>Animal products nec</t>
+    <t>Cereal grains nec</t>
+  </si>
+  <si>
+    <t>Other food, beverages, tobacco</t>
+  </si>
+  <si>
+    <t>Textiles, apparel, furs, leather</t>
+  </si>
+  <si>
+    <t>Cement, lime and plaster</t>
+  </si>
+  <si>
+    <t>Furniture; other manufactured goods n.e.c. (36)</t>
+  </si>
+  <si>
+    <t>Health and social work services (85)</t>
+  </si>
+  <si>
+    <t>Air transport services (62)</t>
+  </si>
+  <si>
+    <t>Post and telecommunication services (64)</t>
+  </si>
+  <si>
+    <t>Recreational, cultural and sporting services (92)</t>
+  </si>
+  <si>
+    <t>Education services (80)</t>
+  </si>
+  <si>
+    <t>Hotel and restaurant services (55)</t>
+  </si>
+  <si>
+    <t>Construction work (45)</t>
+  </si>
+  <si>
+    <t>Dairy products</t>
+  </si>
+  <si>
+    <t>Glass, tiles, ceramics, bricks</t>
+  </si>
+  <si>
+    <t>Office machinery and computers (30)</t>
+  </si>
+  <si>
+    <t>Railway transportation services</t>
+  </si>
+  <si>
+    <t>Computer and related services (72)</t>
+  </si>
+  <si>
+    <t>Printed matter and recorded media (22)</t>
+  </si>
+  <si>
+    <t>Real estate services (70)</t>
+  </si>
+  <si>
+    <t>Meat animals nec</t>
+  </si>
+  <si>
+    <t>Electrical machinery, audiovisual, and medical equipment</t>
+  </si>
+  <si>
+    <t>Wood and products of wood and cork (except furniture); articles of straw and plaiting materials</t>
+  </si>
+  <si>
+    <t>Sea and coastal water transportation services</t>
+  </si>
+  <si>
+    <t>Public administration and defence services; compulsory social security services (75)</t>
+  </si>
+  <si>
+    <t>Meat products</t>
+  </si>
+  <si>
+    <t>Electricity by coal</t>
+  </si>
+  <si>
+    <t>Vehicles and transport equipment</t>
+  </si>
+  <si>
+    <t>Research and development services (73)</t>
+  </si>
+  <si>
+    <t>Paddy rice</t>
+  </si>
+  <si>
+    <t>Electricity by gas and petroleum products</t>
+  </si>
+  <si>
+    <t>Private households with employed persons (95)</t>
+  </si>
+  <si>
+    <t>Other land transportation services</t>
+  </si>
+  <si>
+    <t>Membership organisation services n.e.c. (91)</t>
+  </si>
+  <si>
+    <t>Raw milk</t>
+  </si>
+  <si>
+    <t>Electricity by hydro</t>
+  </si>
+  <si>
+    <t>Other business services (74)</t>
+  </si>
+  <si>
+    <t>Vegetables, fruit, nuts</t>
+  </si>
+  <si>
+    <t>Electricity by nuclear</t>
+  </si>
+  <si>
+    <t>Other services (93)</t>
+  </si>
+  <si>
+    <t>Wheat</t>
+  </si>
+  <si>
+    <t>Electricity by wind</t>
+  </si>
+  <si>
+    <t>Financial intermediation services, insurances</t>
+  </si>
+  <si>
+    <t>products of Vegetable oils and fats</t>
+  </si>
+  <si>
+    <t>Transmission and distribution of electricity</t>
+  </si>
+  <si>
+    <t>Aluminium and aluminium products</t>
+  </si>
+  <si>
+    <t>Crops nec</t>
+  </si>
+  <si>
+    <t>Steam and hot water supply services</t>
+  </si>
+  <si>
+    <t>Composting and land application</t>
+  </si>
+  <si>
+    <t>Fish and other fishing products; services incidental of fishing (05)</t>
+  </si>
+  <si>
+    <t>Natural gas and services related to natural gas extraction, excluding surveying</t>
+  </si>
+  <si>
+    <t>Mining &amp; Quarrying</t>
+  </si>
+  <si>
+    <t>Oil seeds</t>
+  </si>
+  <si>
+    <t>Distribution services of gaseous fuels through mains</t>
+  </si>
+  <si>
+    <t>Landfill</t>
+  </si>
+  <si>
+    <t>Collected and purified water, distribution services of water (41)</t>
+  </si>
+  <si>
+    <t>Produced gas (Gas works, Blast ovens, etc.)</t>
+  </si>
+  <si>
+    <t>Foundry work services</t>
+  </si>
+  <si>
+    <t>Cattle</t>
+  </si>
+  <si>
+    <t>Waste for treatment: biogasification and land application</t>
+  </si>
+  <si>
+    <t>Chemicals nec</t>
   </si>
   <si>
     <t>Biofuels</t>
   </si>
   <si>
-    <t>Textiles, apparel, furs, leather</t>
-  </si>
-  <si>
-    <t>Cement, lime, and plaster</t>
-  </si>
-  <si>
-    <t>Furniture</t>
-  </si>
-  <si>
-    <t>Health and social work services</t>
-  </si>
-  <si>
-    <t>Air transport services</t>
-  </si>
-  <si>
-    <t>Computer and related services</t>
-  </si>
-  <si>
-    <t>Recreational, cultural, and sporting services</t>
-  </si>
-  <si>
-    <t>Education services</t>
-  </si>
-  <si>
-    <t>Hotel and restaurant services</t>
-  </si>
-  <si>
-    <t>Fabricated metal products, except machinery and equipment</t>
-  </si>
-  <si>
-    <t>Cattle</t>
-  </si>
-  <si>
     <t>Coal, peat</t>
   </si>
   <si>
-    <t>Collected and purified water, distribution services of water</t>
-  </si>
-  <si>
-    <t>Glass, tiles, ceramics, bricks</t>
-  </si>
-  <si>
-    <t>Construction work</t>
-  </si>
-  <si>
-    <t>Post and telecommunication services</t>
-  </si>
-  <si>
-    <t>Printed matter and recorded media</t>
-  </si>
-  <si>
-    <t>Financial intermediation services, insurances</t>
-  </si>
-  <si>
-    <t>Cereal grains nec</t>
-  </si>
-  <si>
-    <t>Coke and tar</t>
-  </si>
-  <si>
-    <t>Electricity by coal</t>
-  </si>
-  <si>
-    <t>Office machinery and computers</t>
-  </si>
-  <si>
-    <t>Inland water transportation services</t>
-  </si>
-  <si>
-    <t>Foundry work services</t>
+    <t>Nuclear fuel</t>
+  </si>
+  <si>
+    <t>Coke and Tar</t>
+  </si>
+  <si>
+    <t>Sale, maintenance, repair of motor vehicles, motor vehicles parts, motorcycles, motor cycles parts and accessoiries, fuel stations</t>
+  </si>
+  <si>
+    <t>Pulp</t>
   </si>
   <si>
     <t>Charcoal</t>
   </si>
   <si>
+    <t>Paper and paper products</t>
+  </si>
+  <si>
     <t>Crude petroleum and services related to crude oil extraction, excluding surveying</t>
   </si>
   <si>
-    <t>Electricity by gas and petroleum products</t>
-  </si>
-  <si>
-    <t>Rubber and plastic products</t>
-  </si>
-  <si>
-    <t>Railway transportation services</t>
-  </si>
-  <si>
-    <t>Membership organization services n.e.c.</t>
-  </si>
-  <si>
-    <t>Dairy products</t>
-  </si>
-  <si>
-    <t>Natural gas and services related to natural gas extraction, excluding surveying</t>
-  </si>
-  <si>
-    <t>Electricity by hydro</t>
-  </si>
-  <si>
-    <t>Wood and products of wood and cork (except furniture)</t>
-  </si>
-  <si>
-    <t>Sea and coastal water transportation services</t>
-  </si>
-  <si>
-    <t>Mining &amp; Quarrying</t>
-  </si>
-  <si>
-    <t>Meat animals nec</t>
+    <t>Secondary lead for treatment, Re-processing of secondary lead into new lead</t>
   </si>
   <si>
     <t>Petroleum products</t>
   </si>
   <si>
-    <t>Electricity by nuclear</t>
-  </si>
-  <si>
-    <t>Vehicles and transport equipment</t>
-  </si>
-  <si>
-    <t>Other business services</t>
-  </si>
-  <si>
-    <t>Meat products</t>
-  </si>
-  <si>
-    <t>Other food, beverages, tobacco</t>
-  </si>
-  <si>
-    <t>Electricity by wind</t>
-  </si>
-  <si>
-    <t>Other land transportation services</t>
+    <t>Basic iron and steel and of ferro-alloys and first products thereof</t>
+  </si>
+  <si>
+    <t>Waste incineration</t>
+  </si>
+  <si>
+    <t>Extra-territorial organizations and bodies</t>
+  </si>
+  <si>
+    <t>Fabricated metal products, except machinery and equipment (28)</t>
+  </si>
+  <si>
+    <t>Machinery and equipment n.e.c. (29)</t>
+  </si>
+  <si>
+    <t>N-fertiliser</t>
+  </si>
+  <si>
+    <t>P- and other fertiliser</t>
   </si>
   <si>
     <t>Other metals and products thereof</t>
   </si>
   <si>
-    <t>Oil seeds</t>
-  </si>
-  <si>
-    <t>Steam and hot water supply services</t>
-  </si>
-  <si>
     <t>Other non-metallic mineral products</t>
   </si>
   <si>
-    <t>Paddy rice</t>
-  </si>
-  <si>
-    <t>Transmission and distribution of electricity</t>
-  </si>
-  <si>
-    <t>Other services</t>
-  </si>
-  <si>
-    <t>Products of forestry, logging, and related services</t>
-  </si>
-  <si>
-    <t>Public administration and defense services</t>
-  </si>
-  <si>
-    <t>Products of Vegetable oils and fats</t>
-  </si>
-  <si>
-    <t>Renting services of machinery and equipment without operator and of personal and household goods</t>
-  </si>
-  <si>
-    <t>Vegetables, fruit, nuts</t>
-  </si>
-  <si>
-    <t>Research and development services</t>
-  </si>
-  <si>
-    <t>Wheat</t>
-  </si>
-  <si>
-    <t>Retail trade services, except of motor vehicles and motorcycles; repair services of personal and household goods</t>
-  </si>
-  <si>
-    <t>Sale, maintenance, repair of motor vehicles, motor vehicles parts, motorcycles, motor cycles parts and accessories, fuel stations</t>
-  </si>
-  <si>
-    <t>Secondary lead for treatment, re-processing of secondary lead into new lead</t>
+    <t>Precious metals</t>
+  </si>
+  <si>
+    <t>Products of forestry, logging and related services (02)</t>
+  </si>
+  <si>
+    <t>Renting services of machinery and equipment without operator and of personal and household goods (71)</t>
+  </si>
+  <si>
+    <t>Retail  trade services, except of motor vehicles and motorcycles; repair services of personal and household goods (52)</t>
   </si>
   <si>
     <t>Secondary raw materials</t>
   </si>
   <si>
-    <t>Supporting and auxiliary transport services</t>
+    <t>Supporting and auxiliary transport services; travel agency services (63)</t>
   </si>
   <si>
     <t>Transportation services via pipelines</t>
   </si>
   <si>
-    <t>Waste for treatment: biogasification and land application</t>
-  </si>
-  <si>
-    <t>Waste incineration</t>
-  </si>
-  <si>
-    <t>Wholesale trade and commission trade services, except of motor vehicles and motorcycles</t>
+    <t>Wholesale trade and commission trade services, except of motor vehicles and motorcycles (51)</t>
+  </si>
+  <si>
+    <t>Rubber and plastic products (25)</t>
+  </si>
+  <si>
+    <t>Plastics, basic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -353,8 +462,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,16 +805,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2B5A38-EE05-4B87-B85E-53A18DBAFCC6}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="66.140625" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" customWidth="1"/>
     <col min="4" max="4" width="47.42578125" customWidth="1"/>
     <col min="5" max="5" width="60.7109375" customWidth="1"/>
@@ -711,79 +827,79 @@
     <col min="12" max="12" width="103.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -829,214 +945,309 @@
       <c r="A4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>37</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>38</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>40</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>41</v>
       </c>
-      <c r="I4" t="s">
+      <c r="L4" t="s">
         <v>42</v>
-      </c>
-      <c r="L4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
         <v>44</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>45</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E5" t="s">
+      <c r="L5" t="s">
         <v>47</v>
-      </c>
-      <c r="G5" t="s">
-        <v>48</v>
-      </c>
-      <c r="L5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B6" t="s">
+      <c r="L6" t="s">
         <v>51</v>
-      </c>
-      <c r="D6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" t="s">
-        <v>54</v>
-      </c>
-      <c r="L6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" t="s">
+        <v>55</v>
+      </c>
+      <c r="L7" t="s">
         <v>56</v>
-      </c>
-      <c r="B7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" t="s">
-        <v>60</v>
-      </c>
-      <c r="L7" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="L8" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" t="s">
-        <v>70</v>
-      </c>
-      <c r="L9" t="s">
-        <v>71</v>
+        <v>61</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D10" t="s">
-        <v>73</v>
-      </c>
-      <c r="L10" t="s">
-        <v>74</v>
+        <v>64</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
-      </c>
-      <c r="L11" t="s">
-        <v>77</v>
+        <v>67</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>78</v>
-      </c>
-      <c r="L12" t="s">
-        <v>79</v>
+        <v>69</v>
+      </c>
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>80</v>
-      </c>
-      <c r="L13" t="s">
-        <v>81</v>
+        <v>72</v>
+      </c>
+      <c r="D13" t="s">
+        <v>73</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>75</v>
+      </c>
+      <c r="D14" t="s">
+        <v>76</v>
       </c>
       <c r="L14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" t="s">
+        <v>79</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" t="s">
+        <v>82</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="4:12">
+      <c r="D17" t="s">
         <v>84</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L17" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
-      <c r="L16" t="s">
+    <row r="18" spans="4:12">
+      <c r="D18" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="17" spans="12:12">
-      <c r="L17" t="s">
+      <c r="L18" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="12:12">
-      <c r="L18" t="s">
+    <row r="19" spans="4:12">
+      <c r="D19" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="19" spans="12:12">
-      <c r="L19" t="s">
+      <c r="L19" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="12:12">
+    <row r="20" spans="4:12">
+      <c r="D20" t="s">
+        <v>90</v>
+      </c>
       <c r="L20" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="12:12">
-      <c r="L21" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="12:12">
-      <c r="L22" t="s">
+    <row r="21" spans="4:12">
+      <c r="D21" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="23" spans="12:12">
-      <c r="L23" t="s">
+      <c r="L21" s="1" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="4:12">
+      <c r="D22" t="s">
+        <v>94</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="4:12">
+      <c r="D23" t="s">
+        <v>96</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="4:12">
+      <c r="L24" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="4:12">
+      <c r="L25" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="4:12">
+      <c r="L26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="4:12">
+      <c r="L27" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="4:12">
+      <c r="L28" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="4:12">
+      <c r="L29" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="4:12">
+      <c r="L30" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="4:12">
+      <c r="L31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="4:12">
+      <c r="L32" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="12:12">
+      <c r="L33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="12:12">
+      <c r="L34" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="12:12">
+      <c r="L35" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="12:12">
+      <c r="L36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="12:12">
+      <c r="L37" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="12:12">
+      <c r="L38" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="12:12">
+      <c r="L39" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>